<commit_message>
fix gaz print; add building and montage works calculation {   work values,   work values table calculation; }
</commit_message>
<xml_diff>
--- a/gazPart/documentation/calculation/GazProperties.xlsx
+++ b/gazPart/documentation/calculation/GazProperties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\gazPart\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949BA47-406B-4E8A-A090-C77C115ED2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681D3FE3-F370-485F-A92B-87DF1AB98959}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -2180,17 +2180,17 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>8</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>1.9801077682981592</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2354,13 +2354,13 @@
         <v>1.2523447967842787</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>SUM(B2:B8)</f>
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>0.73337724555280348</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>36021.945</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>14.930213115639303</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>9.6366200000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>9.7037756774560009</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>10.674153245201602</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>1.0125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>2.0052387124520159</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0.2023690200000002</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>8.3802227800000022</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -2498,16 +2498,16 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="12" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
         <v>150</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -2585,7 +2585,7 @@
       <c r="O2" s="108"/>
       <c r="P2" s="110"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>209</v>
       </c>
@@ -2655,7 +2655,7 @@
       <c r="O4" s="83"/>
       <c r="P4" s="84"/>
     </row>
-    <row r="5" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>149.95252768369892</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>146.5021081475951</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>145.64804498602095</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>151.08776506819913</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>164.32258203214897</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>187.03022190536799</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>216.02280431033816</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>262.71281456659369</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>374.29640988436927</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="82" t="s">
         <v>211</v>
       </c>
@@ -3313,7 +3313,7 @@
       <c r="O16" s="83"/>
       <c r="P16" s="84"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>12</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>13</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>0.65</v>
       </c>
       <c r="D18" s="68">
-        <f t="shared" ref="D18:D26" si="8">B18*C18</f>
+        <f t="shared" ref="D18:D25" si="8">B18*C18</f>
         <v>1.4560000000000002</v>
       </c>
       <c r="E18" s="4">
@@ -3428,7 +3428,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>14</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>180.6959633220101</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>15</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>177.24554378590628</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>16</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>176.39148062433213</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>17</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>181.83120070651032</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>18</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>195.06601767046016</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>19</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>217.77365754367918</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>20</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>246.76623994864934</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>21</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>284.28524644416854</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="104" t="s">
         <v>210</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="O27" s="105"/>
       <c r="P27" s="106"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>22</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>23</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>24</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>180.6959633220101</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>177.24554378590628</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>26</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>176.39148062433213</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>27</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>181.83120070651032</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>28</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>195.06601767046016</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>29</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>217.77365754367918</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>30</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>246.76623994864934</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>31</v>
       </c>
@@ -4518,18 +4518,18 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
         <v>150</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="111"/>
       <c r="B2" s="111"/>
       <c r="C2" s="111"/>
@@ -4575,7 +4575,7 @@
       <c r="I2" s="111"/>
       <c r="J2" s="112"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>222</v>
       </c>
@@ -4621,7 +4621,7 @@
       <c r="I4" s="83"/>
       <c r="J4" s="84"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>77.8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>36.14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="82" t="s">
         <v>223</v>
       </c>
@@ -4888,7 +4888,7 @@
       <c r="J11" s="84"/>
       <c r="L11" s="65"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>23.12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>9</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>11</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>13</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5236,7 +5236,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5275,25 +5275,25 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="16" max="16" width="25.85546875" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.88671875" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5450,7 +5450,7 @@
       <c r="T3" s="76"/>
       <c r="U3" s="78"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="T4" s="76"/>
       <c r="U4" s="78"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="T5" s="76"/>
       <c r="U5" s="78"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5567,7 +5567,7 @@
       <c r="T6" s="76"/>
       <c r="U6" s="78"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="T7" s="76"/>
       <c r="U7" s="78"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -5645,7 +5645,7 @@
       <c r="T8" s="76"/>
       <c r="U8" s="78"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="T9" s="76"/>
       <c r="U9" s="78"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5723,7 +5723,7 @@
       <c r="T10" s="76"/>
       <c r="U10" s="78"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -5762,7 +5762,7 @@
       <c r="T11" s="76"/>
       <c r="U11" s="78"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5801,7 +5801,7 @@
       <c r="T12" s="76"/>
       <c r="U12" s="78"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5840,7 +5840,7 @@
       <c r="T13" s="76"/>
       <c r="U13" s="78"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -5879,7 +5879,7 @@
       <c r="T14" s="76"/>
       <c r="U14" s="78"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5918,7 +5918,7 @@
       <c r="T15" s="76"/>
       <c r="U15" s="78"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="T16" s="76"/>
       <c r="U16" s="78"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -5996,7 +5996,7 @@
       <c r="T17" s="76"/>
       <c r="U17" s="78"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -6035,7 +6035,7 @@
       <c r="T18" s="76"/>
       <c r="U18" s="78"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -6074,7 +6074,7 @@
       <c r="T19" s="76"/>
       <c r="U19" s="78"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -6113,7 +6113,7 @@
       <c r="T20" s="76"/>
       <c r="U20" s="78"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -6152,7 +6152,7 @@
       <c r="T21" s="76"/>
       <c r="U21" s="78"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -6191,7 +6191,7 @@
       <c r="T22" s="76"/>
       <c r="U22" s="78"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -6230,7 +6230,7 @@
       <c r="T23" s="76"/>
       <c r="U23" s="78"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -6269,7 +6269,7 @@
       <c r="T24" s="76"/>
       <c r="U24" s="78"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="T25" s="76"/>
       <c r="U25" s="78"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -6347,7 +6347,7 @@
       <c r="T26" s="76"/>
       <c r="U26" s="78"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -6386,7 +6386,7 @@
       <c r="T27" s="76"/>
       <c r="U27" s="78"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -6425,7 +6425,7 @@
       <c r="T28" s="76"/>
       <c r="U28" s="78"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29">
         <f>SUM(C2:C28)</f>
         <v>234.82999999999996</v>
@@ -6491,7 +6491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J30">
         <f>SUMIF($H$2:$H$28,J2,$I$2:$I$28)</f>
         <v>6032</v>
@@ -6533,7 +6533,7 @@
         <v>5057</v>
       </c>
     </row>
-    <row r="33" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K33">
         <f>SUM(K30:N30)</f>
         <v>38239</v>
@@ -6568,9 +6568,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -6663,12 +6663,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -6706,21 +6706,21 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
         <v>42</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="86"/>
       <c r="B2" s="86"/>
       <c r="C2" s="86"/>
@@ -6766,7 +6766,7 @@
       <c r="I2" s="86"/>
       <c r="J2" s="86"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>34</v>
       </c>
@@ -6812,7 +6812,7 @@
       <c r="I4" s="80"/>
       <c r="J4" s="81"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="82" t="s">
         <v>53</v>
       </c>
@@ -6826,7 +6826,7 @@
       <c r="I5" s="83"/>
       <c r="J5" s="84"/>
     </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="L6" s="32"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="83" t="s">
         <v>56</v>
       </c>
@@ -6878,7 +6878,7 @@
       <c r="I7" s="83"/>
       <c r="J7" s="84"/>
     </row>
-    <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>2</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>1264.8223659807281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -6932,7 +6932,7 @@
         <v>1834.8767615750357</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="79" t="s">
         <v>35</v>
       </c>
@@ -6946,7 +6946,7 @@
       <c r="I10" s="80"/>
       <c r="J10" s="81"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="82" t="s">
         <v>53</v>
       </c>
@@ -6960,7 +6960,7 @@
       <c r="I11" s="83"/>
       <c r="J11" s="84"/>
     </row>
-    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>1</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>331.14565685717059</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="83" t="s">
         <v>56</v>
       </c>
@@ -7011,7 +7011,7 @@
       <c r="I13" s="83"/>
       <c r="J13" s="84"/>
     </row>
-    <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>2</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>1050.4187838711782</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -7065,7 +7065,7 @@
         <v>1381.5644407283489</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -7077,7 +7077,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -7089,7 +7089,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
@@ -7105,7 +7105,7 @@
         <v>3216.4412023033847</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -7117,7 +7117,7 @@
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -7129,7 +7129,7 @@
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -7141,7 +7141,7 @@
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -7184,15 +7184,15 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -7216,12 +7216,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E8" s="39" t="s">
         <v>31</v>
       </c>
@@ -7286,7 +7286,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" s="39" t="s">
         <v>69</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>52&amp;"*"&amp;0.05&amp;"*"&amp;'расчетКол-ваЖит'!E29</f>
         <v>52*0.05*79532</v>
@@ -7305,7 +7305,7 @@
         <v>206783.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>79532</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>15.45</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>58</v>
       </c>
@@ -7403,12 +7403,12 @@
         <v>8410</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>3484</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>13935</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -7435,12 +7435,12 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>115</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>118</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>796878</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>44271</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46">
         <f>gazProperties!$B$15</f>
@@ -7525,7 +7525,7 @@
         <v>634698</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>111</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>35261</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>133</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>8054.3176200000007</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>134</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>13258.136</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>135</v>
       </c>
@@ -7580,14 +7580,14 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
         <v>42</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="86"/>
       <c r="B2" s="86"/>
       <c r="C2" s="86"/>
@@ -7633,7 +7633,7 @@
       <c r="I2" s="86"/>
       <c r="J2" s="86"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>90</v>
       </c>
@@ -7679,7 +7679,7 @@
       <c r="I4" s="80"/>
       <c r="J4" s="81"/>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>1</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>47.131763089910272</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>135.50381888349202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>3</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>82.604817893552152</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>4</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>605.33020079843004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="89" t="s">
         <v>108</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="94" t="s">
         <v>91</v>
       </c>
@@ -7845,7 +7845,7 @@
       <c r="I10" s="95"/>
       <c r="J10" s="96"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>1</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>40.299508165554819</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>2</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>351.38649509347704</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>3</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>104.09511017057334</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
         <v>107</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>495.78111342960517</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="79" t="s">
         <v>100</v>
       </c>
@@ -7983,7 +7983,7 @@
       <c r="I15" s="80"/>
       <c r="J15" s="81"/>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="30">
         <v>1</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>85.044125596627694</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="30">
         <v>2</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>106.30515699578461</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>3</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>1449.1166426465866</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="89" t="s">
         <v>106</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>1640.4659252389988</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
@@ -8125,7 +8125,7 @@
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
@@ -8137,7 +8137,7 @@
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="B22" s="43"/>
       <c r="C22" s="43"/>
@@ -8153,7 +8153,7 @@
         <v>3006.8176393339886</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -8165,7 +8165,7 @@
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
@@ -8181,7 +8181,7 @@
         <v>27924.115150059744</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
@@ -8193,7 +8193,7 @@
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="43"/>
       <c r="C26" s="43"/>
@@ -8205,7 +8205,7 @@
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -8217,7 +8217,7 @@
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="43"/>
       <c r="C28" s="43"/>
@@ -8231,15 +8231,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -8250,6 +8241,15 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8264,19 +8264,19 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>125</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -8320,7 +8320,7 @@
       <c r="J2" s="43"/>
       <c r="K2" s="56"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8344,7 +8344,7 @@
       </c>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>1381.5644407283489</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="K6" s="58"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>1640.4659252389988</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -8464,7 +8464,7 @@
       </c>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>11047.236678641313</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="98" t="s">
         <v>136</v>
       </c>
@@ -8505,7 +8505,7 @@
       <c r="I10" s="57"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -8520,7 +8520,7 @@
         <v>14939.837645274045</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -8558,12 +8558,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19">
         <f>B18*1000</f>
         <v>32.179198147696802</v>
@@ -8584,7 +8584,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>273</v>
       </c>
@@ -8606,13 +8606,13 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
         <v>150</v>
       </c>
@@ -8640,7 +8640,7 @@
       </c>
       <c r="J1" s="101"/>
     </row>
-    <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="103"/>
       <c r="B2" s="59" t="s">
         <v>170</v>
@@ -8660,7 +8660,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>160</v>
       </c>
@@ -8706,7 +8706,7 @@
       <c r="I4" s="83"/>
       <c r="J4" s="84"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>161</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>173</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="61" t="s">
         <v>174</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>22331.678700046548</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
         <v>175</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>21341.187429213842</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>176</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>20597.773966286964</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="60" t="s">
         <v>177</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>12274.01255310811</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="60" t="s">
         <v>178</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>1823.3466189261105</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>179</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>1474.6910393793978</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="60" t="s">
         <v>180</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>1474.6910393793978</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="82" t="s">
         <v>171</v>
       </c>
@@ -9078,7 +9078,7 @@
       <c r="I14" s="83"/>
       <c r="J14" s="84"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>161</v>
       </c>
@@ -9117,7 +9117,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="60" t="s">
         <v>162</v>
       </c>
@@ -9157,7 +9157,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="61" t="s">
         <v>163</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>21967.350949225009</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="60" t="s">
         <v>164</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>21618.695369678295</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="61" t="s">
         <v>165</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>11168.029435496295</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>166</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>2844.2680223174393</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="60" t="s">
         <v>167</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>2100.8545593905637</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="60" t="s">
         <v>168</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>1110.3632885578575</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="60" t="s">
         <v>172</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>1110.3632885578575</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="82" t="s">
         <v>183</v>
       </c>
@@ -9451,7 +9451,7 @@
       <c r="I24" s="83"/>
       <c r="J24" s="84"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="82" t="s">
         <v>181</v>
       </c>
@@ -9465,7 +9465,7 @@
       <c r="I25" s="83"/>
       <c r="J25" s="84"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>161</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>31287.380234828255</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="60" t="s">
         <v>162</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>16275.66037780789</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="61" t="s">
         <v>163</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>14432.301601715462</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="60" t="s">
         <v>164</v>
       </c>
@@ -9624,7 +9624,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="61" t="s">
         <v>182</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="82" t="s">
         <v>183</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="I31" s="83"/>
       <c r="J31" s="84"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="82" t="s">
         <v>184</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="I32" s="83"/>
       <c r="J32" s="84"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -9731,7 +9731,7 @@
         <v>31287.380234828255</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="60" t="s">
         <v>173</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>15011.719857020364</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="61" t="s">
         <v>174</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>13623.768257888953</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="60" t="s">
         <v>175</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>11972.946124413229</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="60" t="s">
         <v>176</v>
       </c>
@@ -9891,7 +9891,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="61" t="s">
         <v>185</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="82" t="s">
         <v>186</v>
       </c>
@@ -9945,7 +9945,7 @@
       <c r="I39" s="83"/>
       <c r="J39" s="84"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>180</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>1843.3587760924281</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="60" t="s">
         <v>187</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>498.07365863036836</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="61" t="s">
         <v>182</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="60" t="s">
         <v>185</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="61" t="s">
         <v>188</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>874.59757350808786</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="60" t="s">
         <v>189</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>1650.8221334757231</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="60" t="s">
         <v>172</v>
       </c>
@@ -10226,6 +10226,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A1:A2"/>
@@ -10234,13 +10241,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A32:J32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>